<commit_message>
Update Pertanggal 29 Januari 2024 16:32 WIB
</commit_message>
<xml_diff>
--- a/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblAppObject_MenuAction.xlsx
+++ b/Documentation/Documents/SQL Generator/Data Initial/SysConfig.TblAppObject_MenuAction.xlsx
@@ -5339,10 +5339,10 @@
   <dimension ref="B1:L567"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B553" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B549" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I568" sqref="I568"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2:L567"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>